<commit_message>
Zang.io ----Avaya company 搜集完成
</commit_message>
<xml_diff>
--- a/云产业企业名录.xlsx
+++ b/云产业企业名录.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="云产业公司名目" sheetId="1" r:id="rId1"/>
     <sheet name="创投公司名录" sheetId="2" r:id="rId2"/>
     <sheet name="科技投资网站目录" sheetId="3" r:id="rId3"/>
     <sheet name="其他待研究公司名录" sheetId="4" r:id="rId4"/>
+    <sheet name="新名词新理念" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
   <si>
     <t>企业名录</t>
   </si>
@@ -538,9 +539,6 @@
     <t xml:space="preserve"> Genband launched Kandy i</t>
   </si>
   <si>
-    <t>Avaya built out Zang.io</t>
-  </si>
-  <si>
     <t>http://www.idc.com/</t>
   </si>
   <si>
@@ -554,13 +552,68 @@
   </si>
   <si>
     <t>野狗</t>
+  </si>
+  <si>
+    <t>容联云</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Avaya </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>旗下PAAS服务子公司</t>
+    </r>
+  </si>
+  <si>
+    <t>http://www.zang.io</t>
+  </si>
+  <si>
+    <t>Avaya Zang.io</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+avaya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>从产品提供商到平台提供商的转型布局
+2015年是CPASS的启动年，Zang于2016年成立</t>
+    </r>
+  </si>
+  <si>
+    <t>Zang母公司Avaya：http://www.avaya.com/en/
+Zang产品特性：http://www.zang.io/features
+Zang让Avaya进入平台领域：http://www.nojitter.com/post/240171482/avaya-steps-up-its-platform-game</t>
+  </si>
+  <si>
+    <t>Moxtra</t>
+  </si>
+  <si>
+    <t>Population Health</t>
+  </si>
+  <si>
+    <t>健康医疗</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -598,22 +651,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF3D464D"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="13"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -633,11 +678,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -650,10 +694,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -983,15 +1025,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
@@ -1368,13 +1410,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="24" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1429,23 +1471,57 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="8" t="s">
-        <v>87</v>
+    <row r="27" spans="1:9" ht="75">
+      <c r="A27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" t="s">
+        <v>94</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="16">
+      <c r="A28" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1469,7 +1545,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A27" r:id="rId1"/>
+    <hyperlink ref="A27" r:id="rId1" display="Avaya built out Zang.io"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1535,7 +1611,7 @@
       </c>
     </row>
     <row r="10" spans="1:1" ht="21">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1618,12 +1694,12 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1665,4 +1741,35 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>